<commit_message>
Restrukturierung, Bereineinigung von Code-Redundanzen, Stage 1 von x
Bitte nicht benutzen, es funktioniert noch nichts
</commit_message>
<xml_diff>
--- a/doc/Tagebuch.xlsx
+++ b/doc/Tagebuch.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Datum</t>
   </si>
@@ -132,6 +132,9 @@
   <si>
     <t>- Installation und Anwendung Prettier und PHP-Formatter
 - Bereitstellung Entwicklungstagebuch</t>
+  </si>
+  <si>
+    <t>Restrukturierung, Bereineinigung von Code-Redundanzen, Stage 1 von x</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,6 +770,14 @@
       </c>
       <c r="E16" s="4">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto Setup mit Demo-Daten, Prototyping FormBuilder
- Skripteinbindung für automatische Erstellung benötigter DB-Strukturen
- Erstellung "Setup-Bereich" für Beladen mit Demodaten per Klick
- Prototyping FormBuilder-Klasse für effizienteres Erstellen von Standard-Formularen
</commit_message>
<xml_diff>
--- a/doc/Tagebuch.xlsx
+++ b/doc/Tagebuch.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Datum</t>
   </si>
@@ -167,6 +167,11 @@
 - Dynamische Generierung von Listenanzeigen und Eingabeformularen aus Oberklasse
 - Dynamische Generierung von Listenanzeigen, Create- und Edit-Formularen
 - Dynamische Generierung von Dropdown-Inhalten in Create- und Edit-Formularen</t>
+  </si>
+  <si>
+    <t>- Skripteinbindung für automatische Erstellung benötigter DB-Strukturen
+- Erstellung "Setup-Bereich" für Beladen mit Demodaten per Klick
+- Prototyping FormBuilder-Klasse für effizienteres Erstellen von Standard-Formularen</t>
   </si>
 </sst>
 </file>
@@ -526,11 +531,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +841,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>45152</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:E1"/>

</xml_diff>